<commit_message>
The alpha version is online.
TODO: User manual and tutorial
</commit_message>
<xml_diff>
--- a/samples/BiliBili_danmu.xlsx
+++ b/samples/BiliBili_danmu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hwang/Desktop/repo/VisualDTA/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264F9F90-8F1D-A049-A44E-B38D7547BE5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B7B0AA-13BE-C74C-9B49-27505973E4FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="193">
   <si>
     <t>Proposition</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Dotted Line</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -607,6 +604,9 @@
   </si>
   <si>
     <t>I'm back! I'm noble!</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -997,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2688"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1038,7 +1038,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1046,25 +1046,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
+        <v>192</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1078,13 +1078,13 @@
         <v>44243.970462962963</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1093,7 +1093,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1107,13 +1107,13 @@
         <v>44243.992569444446</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1122,7 +1122,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1136,13 +1136,13 @@
         <v>44244.01798611111</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1165,13 +1165,13 @@
         <v>44244.023252314815</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1194,13 +1194,13 @@
         <v>44244.024837962963</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1209,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1223,13 +1223,13 @@
         <v>44244.02648148148</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1238,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1252,13 +1252,13 @@
         <v>44244.057673611111</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1267,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1281,13 +1281,13 @@
         <v>44244.058206018519</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1296,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1310,13 +1310,13 @@
         <v>44244.060254629629</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1339,13 +1339,13 @@
         <v>44244.060416666667</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1354,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1368,13 +1368,13 @@
         <v>44244.107094907406</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1383,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1397,13 +1397,13 @@
         <v>44244.108749999999</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1412,7 +1412,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1426,13 +1426,13 @@
         <v>44244.113425925927</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1441,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1455,13 +1455,13 @@
         <v>44244.115393518521</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1470,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1484,13 +1484,13 @@
         <v>44244.116157407407</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1499,7 +1499,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1513,13 +1513,13 @@
         <v>44244.12027777778</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1528,7 +1528,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1542,13 +1542,13 @@
         <v>44244.124224537038</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1557,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1571,13 +1571,13 @@
         <v>44244.128946759258</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1586,7 +1586,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1600,13 +1600,13 @@
         <v>44244.263761574075</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1615,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1629,13 +1629,13 @@
         <v>44244.30810185185</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G22">
         <v>2</v>
@@ -1644,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1658,13 +1658,13 @@
         <v>44244.317141203705</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G23">
         <v>2</v>
@@ -1673,7 +1673,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1687,13 +1687,13 @@
         <v>44244.335532407407</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1702,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1716,13 +1716,13 @@
         <v>44244.335995370369</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1731,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1745,13 +1745,13 @@
         <v>44244.336388888885</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1760,7 +1760,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1774,13 +1774,13 @@
         <v>44244.336828703701</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1789,7 +1789,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1803,13 +1803,13 @@
         <v>44244.366180555553</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G28">
         <v>2</v>
@@ -1818,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1832,13 +1832,13 @@
         <v>44245.333553240744</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -1847,7 +1847,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1861,13 +1861,13 @@
         <v>44246.180578703701</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1876,7 +1876,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1890,13 +1890,13 @@
         <v>44246.301296296297</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -1905,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1919,13 +1919,13 @@
         <v>44247.59648148148</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -1934,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1948,13 +1948,13 @@
         <v>44259.205821759257</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G33">
         <v>2</v>
@@ -1963,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -1977,13 +1977,13 @@
         <v>44268.387870370374</v>
       </c>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -1992,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -2006,13 +2006,13 @@
         <v>44268.471851851849</v>
       </c>
       <c r="D35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -2021,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -2035,13 +2035,13 @@
         <v>44243.985925925925</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G36">
         <v>4</v>
@@ -2050,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -2064,13 +2064,13 @@
         <v>44244.038449074076</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G37">
         <v>2</v>
@@ -2079,7 +2079,7 @@
         <v>1</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -2093,13 +2093,13 @@
         <v>44244.096238425926</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -2108,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -2122,13 +2122,13 @@
         <v>44244.203773148147</v>
       </c>
       <c r="D39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -2137,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -2151,13 +2151,13 @@
         <v>44244.237847222219</v>
       </c>
       <c r="D40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -2166,7 +2166,7 @@
         <v>1</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -2180,13 +2180,13 @@
         <v>44244.312627314815</v>
       </c>
       <c r="D41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -2195,7 +2195,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -2209,13 +2209,13 @@
         <v>44244.508113425924</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E42" s="3">
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G42">
         <v>2</v>
@@ -2224,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -2238,13 +2238,13 @@
         <v>44260.25744212963</v>
       </c>
       <c r="D43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E43" s="3">
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -2253,7 +2253,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -2267,13 +2267,13 @@
         <v>44260.298009259262</v>
       </c>
       <c r="D44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G44">
         <v>2</v>
@@ -2282,7 +2282,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -2296,13 +2296,13 @@
         <v>44261.300023148149</v>
       </c>
       <c r="D45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E45" s="3">
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G45">
         <v>2</v>
@@ -2311,7 +2311,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -2325,13 +2325,13 @@
         <v>44261.860231481478</v>
       </c>
       <c r="D46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E46" s="3">
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G46">
         <v>1</v>
@@ -2340,7 +2340,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -2354,13 +2354,13 @@
         <v>44262.127337962964</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E47" s="3">
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G47">
         <v>3</v>
@@ -2369,7 +2369,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -2383,13 +2383,13 @@
         <v>44244.024988425925</v>
       </c>
       <c r="D48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E48" s="3">
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2398,7 +2398,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -2412,13 +2412,13 @@
         <v>44244.038472222222</v>
       </c>
       <c r="D49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E49" s="3">
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2427,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -2441,13 +2441,13 @@
         <v>44244.125798611109</v>
       </c>
       <c r="D50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E50" s="3">
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2456,7 +2456,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -2470,13 +2470,13 @@
         <v>44244.129652777781</v>
       </c>
       <c r="D51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E51" s="3">
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G51">
         <v>1</v>
@@ -2485,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -2499,13 +2499,13 @@
         <v>44244.315115740741</v>
       </c>
       <c r="D52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E52" s="3">
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -2514,7 +2514,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -2528,13 +2528,13 @@
         <v>44244.418287037035</v>
       </c>
       <c r="D53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E53" s="3">
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -2554,13 +2554,13 @@
         <v>44244.684421296297</v>
       </c>
       <c r="D54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E54" s="3">
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G54">
         <v>1</v>
@@ -2580,13 +2580,13 @@
         <v>44244.982152777775</v>
       </c>
       <c r="D55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E55" s="3">
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -2606,13 +2606,13 @@
         <v>44245.343506944446</v>
       </c>
       <c r="D56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E56" s="3">
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G56">
         <v>1</v>
@@ -2632,13 +2632,13 @@
         <v>44247.590312499997</v>
       </c>
       <c r="D57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E57" s="3">
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G57">
         <v>1</v>
@@ -2658,13 +2658,13 @@
         <v>44260.214062500003</v>
       </c>
       <c r="D58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E58" s="3">
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -2684,13 +2684,13 @@
         <v>44244.025138888886</v>
       </c>
       <c r="D59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E59" s="3">
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2710,13 +2710,13 @@
         <v>44244.120405092595</v>
       </c>
       <c r="D60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E60" s="3">
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -2736,13 +2736,13 @@
         <v>44244.31354166667</v>
       </c>
       <c r="D61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E61" s="3">
         <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -2762,13 +2762,13 @@
         <v>44244.400150462963</v>
       </c>
       <c r="D62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G62">
         <v>1</v>
@@ -2788,13 +2788,13 @@
         <v>44259.377592592595</v>
       </c>
       <c r="D63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E63" s="3">
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G63">
         <v>1</v>
@@ -2814,13 +2814,13 @@
         <v>44260.450856481482</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E64" s="3">
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G64">
         <v>1</v>
@@ -2840,13 +2840,13 @@
         <v>44261.636157407411</v>
       </c>
       <c r="D65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E65" s="3">
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G65">
         <v>1</v>
@@ -2866,13 +2866,13 @@
         <v>44262.07303240741</v>
       </c>
       <c r="D66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E66" s="3">
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -2892,13 +2892,13 @@
         <v>44266.570694444446</v>
       </c>
       <c r="D67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E67" s="3">
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -2918,13 +2918,13 @@
         <v>44244.025300925925</v>
       </c>
       <c r="D68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E68" s="3">
         <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -2944,13 +2944,13 @@
         <v>44244.131168981483</v>
       </c>
       <c r="D69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E69" s="3">
         <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G69">
         <v>1</v>
@@ -2970,13 +2970,13 @@
         <v>44244.172789351855</v>
       </c>
       <c r="D70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E70" s="3">
         <v>0</v>
       </c>
       <c r="F70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G70">
         <v>1</v>
@@ -2996,13 +2996,13 @@
         <v>44244.312280092592</v>
       </c>
       <c r="D71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E71" s="3">
         <v>0</v>
       </c>
       <c r="F71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -3022,13 +3022,13 @@
         <v>44244.315960648149</v>
       </c>
       <c r="D72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E72" s="3">
         <v>0</v>
       </c>
       <c r="F72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G72">
         <v>2</v>
@@ -3048,13 +3048,13 @@
         <v>44244.36314814815</v>
       </c>
       <c r="D73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E73" s="3">
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G73">
         <v>1</v>
@@ -3074,13 +3074,13 @@
         <v>44244.438252314816</v>
       </c>
       <c r="D74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E74" s="3">
         <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G74">
         <v>1</v>
@@ -3100,13 +3100,13 @@
         <v>44244.451041666667</v>
       </c>
       <c r="D75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E75" s="3">
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G75">
         <v>1</v>
@@ -3126,13 +3126,13 @@
         <v>44245.448379629626</v>
       </c>
       <c r="D76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E76" s="3">
         <v>0</v>
       </c>
       <c r="F76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G76">
         <v>2</v>
@@ -3152,13 +3152,13 @@
         <v>44247.007094907407</v>
       </c>
       <c r="D77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E77" s="3">
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G77">
         <v>1</v>
@@ -3178,13 +3178,13 @@
         <v>44257.412812499999</v>
       </c>
       <c r="D78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E78" s="3">
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G78">
         <v>1</v>
@@ -3204,13 +3204,13 @@
         <v>44258.058472222219</v>
       </c>
       <c r="D79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E79" s="3">
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G79">
         <v>1</v>
@@ -3230,13 +3230,13 @@
         <v>44259.288472222222</v>
       </c>
       <c r="D80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E80" s="3">
         <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -3256,13 +3256,13 @@
         <v>44261.443368055552</v>
       </c>
       <c r="D81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E81" s="3">
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G81">
         <v>3</v>
@@ -3282,13 +3282,13 @@
         <v>44244.108888888892</v>
       </c>
       <c r="D82" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E82" s="3">
         <v>0</v>
       </c>
       <c r="F82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G82">
         <v>1</v>
@@ -3308,13 +3308,13 @@
         <v>44244.113599537035</v>
       </c>
       <c r="D83" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E83" s="3">
         <v>0</v>
       </c>
       <c r="F83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G83">
         <v>1</v>
@@ -3334,13 +3334,13 @@
         <v>44244.469907407409</v>
       </c>
       <c r="D84" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E84" s="3">
         <v>0</v>
       </c>
       <c r="F84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G84">
         <v>1</v>
@@ -3360,13 +3360,13 @@
         <v>44246.994629629633</v>
       </c>
       <c r="D85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E85" s="3">
         <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G85">
         <v>2</v>
@@ -3386,13 +3386,13 @@
         <v>44261.016481481478</v>
       </c>
       <c r="D86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E86" s="3">
         <v>0</v>
       </c>
       <c r="F86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G86">
         <v>1</v>
@@ -3412,13 +3412,13 @@
         <v>44265.466377314813</v>
       </c>
       <c r="D87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E87" s="3">
         <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G87">
         <v>1</v>
@@ -3438,13 +3438,13 @@
         <v>44266.287349537037</v>
       </c>
       <c r="D88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E88" s="3">
         <v>0</v>
       </c>
       <c r="F88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G88">
         <v>1</v>
@@ -3464,13 +3464,13 @@
         <v>44268.020451388889</v>
       </c>
       <c r="D89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E89" s="3">
         <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G89">
         <v>2</v>
@@ -3490,13 +3490,13 @@
         <v>44268.078634259262</v>
       </c>
       <c r="D90" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E90" s="3">
         <v>0</v>
       </c>
       <c r="F90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G90">
         <v>1</v>
@@ -3516,13 +3516,13 @@
         <v>44268.231585648151</v>
       </c>
       <c r="D91" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E91" s="3">
         <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G91">
         <v>1</v>
@@ -3542,13 +3542,13 @@
         <v>44244.062337962961</v>
       </c>
       <c r="D92" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E92" s="3">
         <v>0</v>
       </c>
       <c r="F92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G92">
         <v>1</v>
@@ -3568,13 +3568,13 @@
         <v>44244.120520833334</v>
       </c>
       <c r="D93" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E93" s="3">
         <v>0</v>
       </c>
       <c r="F93" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -3594,13 +3594,13 @@
         <v>44244.122245370374</v>
       </c>
       <c r="D94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E94" s="3">
         <v>0</v>
       </c>
       <c r="F94" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -3620,13 +3620,13 @@
         <v>44244.313009259262</v>
       </c>
       <c r="D95" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E95" s="3">
         <v>0</v>
       </c>
       <c r="F95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G95">
         <v>1</v>
@@ -3646,13 +3646,13 @@
         <v>44244.317604166667</v>
       </c>
       <c r="D96" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E96" s="3">
         <v>0</v>
       </c>
       <c r="F96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G96">
         <v>1</v>
@@ -3672,13 +3672,13 @@
         <v>44245.407361111109</v>
       </c>
       <c r="D97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E97" s="3">
         <v>0</v>
       </c>
       <c r="F97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G97">
         <v>1</v>
@@ -3698,13 +3698,13 @@
         <v>44246.539560185185</v>
       </c>
       <c r="D98" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E98" s="3">
         <v>0</v>
       </c>
       <c r="F98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G98">
         <v>2</v>
@@ -3724,13 +3724,13 @@
         <v>44260.215300925927</v>
       </c>
       <c r="D99" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E99" s="3">
         <v>0</v>
       </c>
       <c r="F99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G99">
         <v>2</v>
@@ -3750,13 +3750,13 @@
         <v>44260.510289351849</v>
       </c>
       <c r="D100" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E100" s="3">
         <v>0</v>
       </c>
       <c r="F100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G100">
         <v>1</v>
@@ -3776,13 +3776,13 @@
         <v>44261.442395833335</v>
       </c>
       <c r="D101" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E101" s="3">
         <v>0</v>
       </c>
       <c r="F101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G101">
         <v>3</v>
@@ -3802,13 +3802,13 @@
         <v>44268.943379629629</v>
       </c>
       <c r="D102" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E102" s="3">
         <v>0</v>
       </c>
       <c r="F102" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G102">
         <v>1</v>
@@ -3828,13 +3828,13 @@
         <v>44243.959560185183</v>
       </c>
       <c r="D103" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E103" s="3">
         <v>0</v>
       </c>
       <c r="F103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G103">
         <v>1</v>
@@ -3854,13 +3854,13 @@
         <v>44244.022013888891</v>
       </c>
       <c r="D104" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E104" s="3">
         <v>0</v>
       </c>
       <c r="F104" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -3880,13 +3880,13 @@
         <v>44244.028993055559</v>
       </c>
       <c r="D105" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E105" s="3">
         <v>0</v>
       </c>
       <c r="F105" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -3906,13 +3906,13 @@
         <v>44244.124409722222</v>
       </c>
       <c r="D106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E106" s="3">
         <v>0</v>
       </c>
       <c r="F106" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -3932,13 +3932,13 @@
         <v>44244.125300925924</v>
       </c>
       <c r="D107" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E107" s="3">
         <v>0</v>
       </c>
       <c r="F107" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G107">
         <v>1</v>
@@ -3958,13 +3958,13 @@
         <v>44244.9059375</v>
       </c>
       <c r="D108" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E108" s="3">
         <v>0</v>
       </c>
       <c r="F108" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G108">
         <v>3</v>
@@ -3984,13 +3984,13 @@
         <v>44257.413263888891</v>
       </c>
       <c r="D109" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E109">
         <v>0</v>
       </c>
       <c r="F109" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G109">
         <v>2</v>
@@ -4010,13 +4010,13 @@
         <v>44259.442858796298</v>
       </c>
       <c r="D110" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E110" s="3">
         <v>0</v>
       </c>
       <c r="F110" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -4036,13 +4036,13 @@
         <v>44260.146770833337</v>
       </c>
       <c r="D111" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E111" s="3">
         <v>0</v>
       </c>
       <c r="F111" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -4062,13 +4062,13 @@
         <v>44244.181585648148</v>
       </c>
       <c r="D112" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E112" s="3">
         <v>0</v>
       </c>
       <c r="F112" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G112">
         <v>2</v>
@@ -4088,13 +4088,13 @@
         <v>44244.484259259261</v>
       </c>
       <c r="D113" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E113" s="3">
         <v>0</v>
       </c>
       <c r="F113" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G113">
         <v>1</v>
@@ -4114,13 +4114,13 @@
         <v>44245.178657407407</v>
       </c>
       <c r="D114" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E114" s="3">
         <v>0</v>
       </c>
       <c r="F114" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G114">
         <v>2</v>
@@ -4140,13 +4140,13 @@
         <v>44260.420810185184</v>
       </c>
       <c r="D115" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E115" s="3">
         <v>0</v>
       </c>
       <c r="F115" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G115">
         <v>1</v>
@@ -4166,13 +4166,13 @@
         <v>44261.133657407408</v>
       </c>
       <c r="D116" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E116" s="3">
         <v>0</v>
       </c>
       <c r="F116" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G116">
         <v>1</v>
@@ -4192,13 +4192,13 @@
         <v>44264.393043981479</v>
       </c>
       <c r="D117" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E117" s="3">
         <v>0</v>
       </c>
       <c r="F117" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G117">
         <v>2</v>
@@ -4218,13 +4218,13 @@
         <v>44243.99324074074</v>
       </c>
       <c r="D118" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E118" s="3">
         <v>0</v>
       </c>
       <c r="F118" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -4244,13 +4244,13 @@
         <v>44244.122986111113</v>
       </c>
       <c r="D119" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E119" s="3">
         <v>0</v>
       </c>
       <c r="F119" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G119">
         <v>2</v>
@@ -4270,13 +4270,13 @@
         <v>44244.317280092589</v>
       </c>
       <c r="D120" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E120" s="3">
         <v>0</v>
       </c>
       <c r="F120" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -4296,13 +4296,13 @@
         <v>44244.721087962964</v>
       </c>
       <c r="D121" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E121" s="3">
         <v>0</v>
       </c>
       <c r="F121" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G121">
         <v>2</v>
@@ -4322,13 +4322,13 @@
         <v>44245.238877314812</v>
       </c>
       <c r="D122" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E122" s="3">
         <v>0</v>
       </c>
       <c r="F122" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -4348,13 +4348,13 @@
         <v>44257.509791666664</v>
       </c>
       <c r="D123" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E123" s="3">
         <v>0</v>
       </c>
       <c r="F123" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G123">
         <v>1</v>
@@ -4374,13 +4374,13 @@
         <v>44260.026828703703</v>
       </c>
       <c r="D124" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E124" s="3">
         <v>0</v>
       </c>
       <c r="F124" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G124">
         <v>2</v>
@@ -4400,13 +4400,13 @@
         <v>44261.827650462961</v>
       </c>
       <c r="D125" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E125" s="3">
         <v>0</v>
       </c>
       <c r="F125" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G125">
         <v>1</v>
@@ -4426,13 +4426,13 @@
         <v>44262.989768518521</v>
       </c>
       <c r="D126" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E126" s="3">
         <v>0</v>
       </c>
       <c r="F126" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G126">
         <v>1</v>
@@ -4452,13 +4452,13 @@
         <v>44266.742743055554</v>
       </c>
       <c r="D127" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E127" s="3">
         <v>0</v>
       </c>
       <c r="F127" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G127">
         <v>1</v>
@@ -4478,13 +4478,13 @@
         <v>44244.180115740739</v>
       </c>
       <c r="D128" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E128" s="3">
         <v>0</v>
       </c>
       <c r="F128" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G128">
         <v>1</v>
@@ -4504,13 +4504,13 @@
         <v>44246.146145833336</v>
       </c>
       <c r="D129" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E129" s="3">
         <v>0</v>
       </c>
       <c r="F129" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G129">
         <v>2</v>
@@ -4530,13 +4530,13 @@
         <v>44247.087500000001</v>
       </c>
       <c r="D130" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E130" s="3">
         <v>0</v>
       </c>
       <c r="F130" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G130">
         <v>0</v>
@@ -4556,13 +4556,13 @@
         <v>44258.760196759256</v>
       </c>
       <c r="D131" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E131" s="3">
         <v>0</v>
       </c>
       <c r="F131" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G131">
         <v>2</v>
@@ -4582,13 +4582,13 @@
         <v>44268.505914351852</v>
       </c>
       <c r="D132" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E132" s="3">
         <v>0</v>
       </c>
       <c r="F132" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G132">
         <v>1</v>

</xml_diff>